<commit_message>
New version of lci concrete with uncertainties
</commit_message>
<xml_diff>
--- a/lci-concrete-with-uncertainties.xlsx
+++ b/lci-concrete-with-uncertainties.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navaroap\autumn-school-bw2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucille.baucal-poyac\Desktop\Documents CETU\Formations\2023-10-09 Formation Brigthway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B52340E-E79F-4F83-A6BF-129C7F2D4CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016"/>
   </bookViews>
   <sheets>
     <sheet name="lci-concrete" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
   <si>
     <t>Database</t>
   </si>
@@ -183,12 +182,15 @@
   </si>
   <si>
     <t>scale</t>
+  </si>
+  <si>
+    <t>concrete production, 25 MPa, all types cement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -989,11 +991,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,7 +1038,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1097,7 +1099,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1115,7 +1117,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1147,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J24" si="0">LN(B12)</f>
+        <f t="shared" ref="J12:J23" si="0">LN(B12)</f>
         <v>5.6698809229805196</v>
       </c>
       <c r="K12">

</xml_diff>